<commit_message>
Completando archivo resumen de performance
</commit_message>
<xml_diff>
--- a/German/Resumen performance.xlsx
+++ b/German/Resumen performance.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C17A61-0434-4383-BC7A-16693D062092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD695AF-776C-43B5-A94C-68E8383FD617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primera Competencia" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>N° intento</t>
   </si>
@@ -63,13 +60,54 @@
   </si>
   <si>
     <t>Media</t>
+  </si>
+  <si>
+    <t>Primer Modelo dado en clase 1, con calculo propio previo de "clase_ternaria"</t>
+  </si>
+  <si>
+    <t>Segunda mejor solución del gridsearch propio de la clase 2</t>
+  </si>
+  <si>
+    <t>Primer mejor solución del gridsearch propio de la clase 2</t>
+  </si>
+  <si>
+    <t>Tercer mejor solución del gridsearch propio de la clase 2</t>
+  </si>
+  <si>
+    <t>Cuarta mejor solución del gridsearch propio de la clase 2</t>
+  </si>
+  <si>
+    <t>Quinta mejor solución del gridsearch propio de la clase 2</t>
+  </si>
+  <si>
+    <t>Primer mejor optimización bayesiana de la clase 3</t>
+  </si>
+  <si>
+    <t>Segunda mejor optimización bayesiana de la clase 3</t>
+  </si>
+  <si>
+    <t>Tercera mejor optimización bayesiana de la clase 3</t>
+  </si>
+  <si>
+    <t>Cuarta mejor optimización bayesiana de la clase 3</t>
+  </si>
+  <si>
+    <t>Quinta mejor optimización bayesiana de la clase 3</t>
+  </si>
+  <si>
+    <t>Competencia_01 (mal solución)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="167" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="175" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,13 +126,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,17 +164,17 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,8 +211,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -189,64 +226,151 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -305,6 +429,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15040181097906052"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -314,9 +446,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1224136286869065"/>
-          <c:y val="0.11218823056953946"/>
-          <c:w val="0.85425682570663386"/>
+          <c:x val="8.8457771301507518E-2"/>
+          <c:y val="0.13040316681726261"/>
+          <c:w val="0.87915778778925979"/>
           <c:h val="0.79354531503234227"/>
         </c:manualLayout>
       </c:layout>
@@ -328,7 +460,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Primera Competencia'!$C$1</c:f>
+              <c:f>'Primera Competencia'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -349,21 +481,21 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Primera Competencia'!$A$3:$A$20</c:f>
+              <c:f>'Primera Competencia'!$B$3:$B$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -384,35 +516,74 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Primera Competencia'!$C$3:$C$20</c:f>
+              <c:f>'Primera Competencia'!$D$3:$D$19</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>86.258667000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>85.194666999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85.134</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.134</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.471333000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000">
+                  <c:v>82.195400000000006</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.0000">
+                  <c:v>73.354399999999998</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0000">
+                  <c:v>66.252200000000002</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.0000">
+                  <c:v>80.047799999999995</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.0000">
+                  <c:v>66.299800000000005</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.0000">
+                  <c:v>67.213999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.0000">
+                  <c:v>66.206000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.0000">
+                  <c:v>64.134</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.0000">
+                  <c:v>63.821333000000003</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.0000">
+                  <c:v>63.821333000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -428,7 +599,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Primera Competencia'!$D$1:$D$2</c:f>
+              <c:f>'Primera Competencia'!$E$1:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -438,26 +609,33 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Primera Competencia'!$A$3:$A$20</c:f>
+              <c:f>'Primera Competencia'!$B$3:$B$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -478,35 +656,74 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Primera Competencia'!$D$3:$D$20</c:f>
+              <c:f>'Primera Competencia'!$E$3:$E$19</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>21.746500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.359639999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.932929999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49.932929999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.933160000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.792990000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.792990000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.746319999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.286369999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47.086289999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44.449649999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>47.226289999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47.809620000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.926279999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47.926279999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -556,7 +773,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -586,6 +803,7 @@
         <c:axId val="1819361754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -642,9 +860,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10708126679411253"/>
-          <c:y val="0.64983118913414517"/>
-          <c:w val="0.35472552348613468"/>
+          <c:x val="0.62321029905217695"/>
+          <c:y val="0.16531388494470975"/>
+          <c:w val="0.34567062818336158"/>
           <c:h val="0.19035669721612672"/>
         </c:manualLayout>
       </c:layout>
@@ -687,9 +905,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>45062</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>203385</xdr:rowOff>
+      <xdr:colOff>371633</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>153039</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5610225" cy="3486150"/>
     <xdr:graphicFrame macro="">
@@ -718,267 +936,6 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Scores"/>
-      <sheetName val="Desc 8"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="C1" t="str">
-            <v>Score Interno</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>Score 
-Kaggle Público</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>1</v>
-          </cell>
-          <cell r="C3">
-            <v>181479.61199999999</v>
-          </cell>
-          <cell r="E3">
-            <v>482297.00244000001</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>2</v>
-          </cell>
-          <cell r="C4">
-            <v>368715</v>
-          </cell>
-          <cell r="E4">
-            <v>379887.85772999999</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>3</v>
-          </cell>
-          <cell r="C5">
-            <v>362382.08000000002</v>
-          </cell>
-          <cell r="E5">
-            <v>385892.69183000003</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>4</v>
-          </cell>
-          <cell r="C6">
-            <v>361055.59</v>
-          </cell>
-          <cell r="E6">
-            <v>350988.34247999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>5</v>
-          </cell>
-          <cell r="C7">
-            <v>355343.125</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>6</v>
-          </cell>
-          <cell r="C8">
-            <v>355343.125</v>
-          </cell>
-          <cell r="E8">
-            <v>337127.42025000002</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>7</v>
-          </cell>
-          <cell r="C9">
-            <v>355706.84</v>
-          </cell>
-          <cell r="E9">
-            <v>326602.31211</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>8</v>
-          </cell>
-          <cell r="C10">
-            <v>206971.00034999999</v>
-          </cell>
-          <cell r="E10">
-            <v>292717.02097000001</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>9</v>
-          </cell>
-          <cell r="C11">
-            <v>197664.178224</v>
-          </cell>
-          <cell r="E11">
-            <v>288474.54806</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>10</v>
-          </cell>
-          <cell r="C12">
-            <v>181281.26761499999</v>
-          </cell>
-          <cell r="E12">
-            <v>293267.41545999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>11</v>
-          </cell>
-          <cell r="C13">
-            <v>196290.035787</v>
-          </cell>
-          <cell r="E13">
-            <v>343964.17249000003</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>12</v>
-          </cell>
-          <cell r="C14">
-            <v>195926.92042800001</v>
-          </cell>
-          <cell r="E14">
-            <v>270515.16723999998</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>13</v>
-          </cell>
-          <cell r="C15">
-            <v>124944.0088</v>
-          </cell>
-          <cell r="E15">
-            <v>263115.08863000001</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>14</v>
-          </cell>
-          <cell r="C16">
-            <v>124463.86870000001</v>
-          </cell>
-          <cell r="E16">
-            <v>263620.96798000002</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>15</v>
-          </cell>
-          <cell r="C17">
-            <v>124590.84790000001</v>
-          </cell>
-          <cell r="E17">
-            <v>264625.90292000002</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>16</v>
-          </cell>
-          <cell r="C18">
-            <v>123408.35410000001</v>
-          </cell>
-          <cell r="E18">
-            <v>264385.65292999998</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19">
-            <v>282435.61959999998</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>17</v>
-          </cell>
-          <cell r="C20">
-            <v>124551.16690000001</v>
-          </cell>
-          <cell r="E20">
-            <v>261682.44393000001</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>18</v>
-          </cell>
-          <cell r="C21">
-            <v>143637.36582000001</v>
-          </cell>
-          <cell r="E21">
-            <v>257929.88394999999</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>19</v>
-          </cell>
-          <cell r="C22">
-            <v>124574.9755</v>
-          </cell>
-          <cell r="E22">
-            <v>261528.52565</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>20</v>
-          </cell>
-          <cell r="C23">
-            <v>157182.46779999998</v>
-          </cell>
-          <cell r="E23">
-            <v>246223.50802000001</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>21</v>
-          </cell>
-          <cell r="C24">
-            <v>41055.4127587857</v>
-          </cell>
-          <cell r="E24">
-            <v>271992.22272000002</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1244,249 +1201,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10:L11"/>
+      <selection pane="bottomRight" activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.5703125" style="1"/>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="1"/>
+    <col min="3" max="3" width="65.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="25.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="E2" s="6"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="22">
+        <v>34.41639</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="19">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="35">
+        <v>86.258667000000003</v>
+      </c>
+      <c r="E4" s="23">
+        <v>21.746500000000001</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="36">
+        <v>85.194666999999995</v>
+      </c>
+      <c r="E5" s="24">
+        <v>45.359639999999999</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="20">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="C6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="36">
+        <v>85.134</v>
+      </c>
+      <c r="E6" s="24">
+        <v>49.932929999999999</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="20">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="C7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="37">
+        <v>85.134</v>
+      </c>
+      <c r="E7" s="24">
+        <v>49.932929999999999</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="21">
         <v>6</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="C8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="38">
+        <v>84.471333000000001</v>
+      </c>
+      <c r="E8" s="25">
+        <v>21.933160000000001</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="19">
         <v>7</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="C9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="31">
+        <v>82.195400000000006</v>
+      </c>
+      <c r="E9" s="23">
+        <v>42.792990000000003</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="20">
         <v>8</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="C10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="32">
+        <v>73.354399999999998</v>
+      </c>
+      <c r="E10" s="24">
+        <v>42.792990000000003</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="20">
         <v>9</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="C11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="32">
+        <v>66.252200000000002</v>
+      </c>
+      <c r="E11" s="24">
+        <v>42.746319999999997</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="20">
         <v>10</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="C12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="33">
+        <v>80.047799999999995</v>
+      </c>
+      <c r="E12" s="24">
+        <v>37.286369999999998</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="21">
         <v>11</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="C13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="34">
+        <v>66.299800000000005</v>
+      </c>
+      <c r="E13" s="25">
+        <v>47.086289999999998</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="18">
         <v>12</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="22">
+        <v>40.273009999999999</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="19">
         <v>13</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="C15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="31">
+        <v>67.213999999999999</v>
+      </c>
+      <c r="E15" s="23">
+        <v>44.449649999999998</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="20">
         <v>14</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="C16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="32">
+        <v>66.206000000000003</v>
+      </c>
+      <c r="E16" s="24">
+        <v>47.226289999999999</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="20">
         <v>15</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="C17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="32">
+        <v>64.134</v>
+      </c>
+      <c r="E17" s="24">
+        <v>47.809620000000002</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="20">
         <v>16</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="C18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="33">
+        <v>63.821333000000003</v>
+      </c>
+      <c r="E18" s="24">
+        <v>47.926279999999998</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="21">
         <v>17</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="C19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="34">
+        <v>63.821333000000003</v>
+      </c>
+      <c r="E19" s="25">
+        <v>47.926279999999998</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="19">
         <v>18</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="C23" s="14"/>
+      <c r="C20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="31"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="20">
+        <v>19</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="32"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="20">
+        <v>20</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="20">
+        <v>21</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="33"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="21">
+        <v>22</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="34"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Armado de esqueleto de estímulos de envíos
</commit_message>
<xml_diff>
--- a/German/Resumen performance.xlsx
+++ b/German/Resumen performance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6A1A4C-FF0E-4C8A-B4E0-407FA3D30166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29784495-99D5-42CE-ACD7-E71727EB4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primera Competencia" sheetId="1" r:id="rId1"/>
+    <sheet name="En búsqueda de la meseta" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>N° intento</t>
   </si>
@@ -96,6 +97,15 @@
   </si>
   <si>
     <t>Competencia_01 (mal solución)</t>
+  </si>
+  <si>
+    <t>Estímulos</t>
+  </si>
+  <si>
+    <t>Public Score</t>
+  </si>
+  <si>
+    <t>Solución 18: Primer mejor optimización bayesiana de la clase 3</t>
   </si>
 </sst>
 </file>
@@ -274,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -365,6 +375,27 @@
     <xf numFmtId="164" fontId="10" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -383,27 +414,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2261,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A25" sqref="A25:G25"/>
@@ -2280,37 +2291,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="39" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="33"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="41" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="11">
@@ -2327,7 +2338,7 @@
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -2347,7 +2358,7 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -2367,7 +2378,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -2387,7 +2398,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="11">
         <v>5</v>
       </c>
@@ -2407,7 +2418,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="13">
         <v>6</v>
       </c>
@@ -2427,7 +2438,7 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -2447,7 +2458,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -2467,7 +2478,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="11">
         <v>9</v>
       </c>
@@ -2487,7 +2498,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -2507,7 +2518,7 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="13">
         <v>11</v>
       </c>
@@ -2737,22 +2748,22 @@
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="39">
+      <c r="A25" s="32"/>
+      <c r="B25" s="33">
         <v>23</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="42">
+      <c r="D25" s="35"/>
+      <c r="E25" s="36">
         <v>40.273009999999999</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="37">
         <f t="shared" ref="F25" si="1">+D25-E25</f>
         <v>-40.273009999999999</v>
       </c>
-      <c r="G25" s="44"/>
+      <c r="G25" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2768,4 +2779,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40565344-81F6-4F0B-A109-33F94B976C9A}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="45">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="45">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="45">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="45">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="45">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="45">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="45">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="45">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="45">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="45">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="45">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="45">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="45">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="45">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="45">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="45">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="45">
+        <v>11500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="45">
+        <v>12000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modelo final de experimentos
</commit_message>
<xml_diff>
--- a/German/Resumen performance.xlsx
+++ b/German/Resumen performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29784495-99D5-42CE-ACD7-E71727EB4499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205B3E16-DF11-49DF-83A3-BB3AAD3A72AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>N° intento</t>
   </si>
@@ -107,17 +107,75 @@
   <si>
     <t>Solución 18: Primer mejor optimización bayesiana de la clase 3</t>
   </si>
+  <si>
+    <t>sol-24</t>
+  </si>
+  <si>
+    <t>sol-25</t>
+  </si>
+  <si>
+    <t>sol-26</t>
+  </si>
+  <si>
+    <t>sol-27</t>
+  </si>
+  <si>
+    <t>sol-28</t>
+  </si>
+  <si>
+    <t>sol-29</t>
+  </si>
+  <si>
+    <t>sol-30</t>
+  </si>
+  <si>
+    <t>sol-31</t>
+  </si>
+  <si>
+    <t>sol-32</t>
+  </si>
+  <si>
+    <t>sol-33</t>
+  </si>
+  <si>
+    <t>sol-34</t>
+  </si>
+  <si>
+    <t>sol-35</t>
+  </si>
+  <si>
+    <t>sol-36</t>
+  </si>
+  <si>
+    <t>sol-37</t>
+  </si>
+  <si>
+    <t>sol-38</t>
+  </si>
+  <si>
+    <t>sol-39</t>
+  </si>
+  <si>
+    <t>sol-40</t>
+  </si>
+  <si>
+    <t>sol-41</t>
+  </si>
+  <si>
+    <t>sol-42</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +246,14 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -284,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -396,6 +462,7 @@
     <xf numFmtId="3" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -414,7 +481,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1375,6 +1445,588 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050"/>
+              <a:t>Public</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" baseline="0"/>
+              <a:t> Score de Kaggle y </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050"/>
+              <a:t>Cantidad</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" baseline="0"/>
+              <a:t> de Estímulos Enviados </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19808333333333333"/>
+          <c:y val="2.3148148148148147E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10126159230096236"/>
+          <c:y val="0.11152777777777778"/>
+          <c:w val="0.86818285214348201"/>
+          <c:h val="0.68206911636045497"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'En búsqueda de la meseta'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Public Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'En búsqueda de la meseta'!$B$3:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'En búsqueda de la meseta'!$C$3:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>37.706359999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.573009999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48.159610000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.646279999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45.102969999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.04627</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.196249999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49.699599999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.242910000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.756239999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.07958</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51.636249999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.232939999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>47.926279999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48.20628</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.349600000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>48.486280000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>47.342959999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>42.699660000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D47-4766-9CC8-A146C4A1B65D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="942592416"/>
+        <c:axId val="11533312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="942592416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Estímulos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11533312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="11533312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="35"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-AR"/>
+                  <a:t>Public Score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-AR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="942592416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1415,7 +2067,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1999,6 +3207,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>257181</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19056</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>257181</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95256</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7CBA17A-FBC6-1EFC-3D57-6D54C19C1920}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2276,7 +3525,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25:G25"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2291,37 +3540,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="40" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="11">
@@ -2338,7 +3587,7 @@
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="42"/>
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -2358,7 +3607,7 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="42"/>
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -2378,7 +3627,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -2398,7 +3647,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="11">
         <v>5</v>
       </c>
@@ -2418,7 +3667,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="13">
         <v>6</v>
       </c>
@@ -2438,7 +3687,7 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -2458,7 +3707,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -2478,7 +3727,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="11">
         <v>9</v>
       </c>
@@ -2498,7 +3747,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -2518,7 +3767,7 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="13">
         <v>11</v>
       </c>
@@ -2786,19 +4035,22 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="7.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="47" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2811,101 +4063,217 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="45">
+      <c r="A3" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="39">
         <v>2000</v>
       </c>
+      <c r="C3" s="46">
+        <v>37.706359999999997</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="45">
+      <c r="A4" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="39">
         <v>3000</v>
       </c>
+      <c r="C4" s="46">
+        <v>39.573009999999996</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="45">
+      <c r="A5" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="39">
         <v>4000</v>
       </c>
+      <c r="C5" s="46">
+        <v>48.159610000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="45">
+      <c r="A6" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="39">
         <v>4500</v>
       </c>
+      <c r="C6" s="46">
+        <v>47.646279999999997</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="45">
+      <c r="A7" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="39">
         <v>5000</v>
       </c>
+      <c r="C7" s="46">
+        <v>45.102969999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="45">
+      <c r="A8" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="39">
         <v>5500</v>
       </c>
+      <c r="C8" s="46">
+        <v>49.04627</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="45">
+      <c r="A9" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="39">
         <v>6000</v>
       </c>
+      <c r="C9" s="46">
+        <v>52.196249999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="45">
+      <c r="A10" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="39">
         <v>6500</v>
       </c>
+      <c r="C10" s="46">
+        <v>49.699599999999997</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="45">
+      <c r="A11" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="39">
         <v>7000</v>
       </c>
+      <c r="C11" s="46">
+        <v>52.242910000000002</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="45">
+      <c r="A12" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="39">
         <v>7500</v>
       </c>
+      <c r="C12" s="46">
+        <v>52.756239999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="45">
+      <c r="A13" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="39">
         <v>8000</v>
       </c>
+      <c r="C13" s="46">
+        <v>52.07958</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
+      <c r="A14" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="39">
         <v>8500</v>
       </c>
+      <c r="C14" s="46">
+        <v>51.636249999999997</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="45">
+      <c r="A15" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="39">
         <v>9000</v>
       </c>
+      <c r="C15" s="46">
+        <v>49.232939999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="45">
+      <c r="A16" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="39">
         <v>9500</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="45">
+      <c r="C16" s="46">
+        <v>47.926279999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="39">
         <v>10000</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45">
+      <c r="C17" s="46">
+        <v>48.20628</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="39">
         <v>10500</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="45">
+      <c r="C18" s="46">
+        <v>49.349600000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="39">
         <v>11500</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45">
-        <v>12000</v>
+      <c r="C19" s="46">
+        <v>48.486280000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="39">
+        <v>13000</v>
+      </c>
+      <c r="C20" s="46">
+        <v>47.342959999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="39">
+        <v>15000</v>
+      </c>
+      <c r="C21" s="46">
+        <v>42.699660000000002</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Terminado en búsqueda de la meseta
</commit_message>
<xml_diff>
--- a/German/Resumen performance.xlsx
+++ b/German/Resumen performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205B3E16-DF11-49DF-83A3-BB3AAD3A72AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96698562-D113-44A8-AB22-7F6B15A743A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -463,6 +463,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -481,10 +485,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1837,7 +1837,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3540,37 +3540,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="42" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="41"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="1:7" ht="15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="11">
@@ -3587,7 +3587,7 @@
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="12">
         <v>2</v>
       </c>
@@ -3607,7 +3607,7 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -3627,7 +3627,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="42"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -3647,7 +3647,7 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="11">
         <v>5</v>
       </c>
@@ -3667,7 +3667,7 @@
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="13">
         <v>6</v>
       </c>
@@ -3687,7 +3687,7 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="42"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="12">
         <v>7</v>
       </c>
@@ -3707,7 +3707,7 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -3727,7 +3727,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="11">
         <v>9</v>
       </c>
@@ -3747,7 +3747,7 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -3767,7 +3767,7 @@
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="13">
         <v>11</v>
       </c>
@@ -4050,7 +4050,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="41" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4063,211 +4063,211 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="41" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="39">
         <v>2000</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="40">
         <v>37.706359999999997</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="41" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="39">
         <v>3000</v>
       </c>
-      <c r="C4" s="46">
+      <c r="C4" s="40">
         <v>39.573009999999996</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="41" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="39">
         <v>4000</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="40">
         <v>48.159610000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="41" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="39">
         <v>4500</v>
       </c>
-      <c r="C6" s="46">
+      <c r="C6" s="40">
         <v>47.646279999999997</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="41" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="39">
         <v>5000</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="40">
         <v>45.102969999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="41" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="39">
         <v>5500</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="40">
         <v>49.04627</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="41" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="39">
         <v>6000</v>
       </c>
-      <c r="C9" s="46">
+      <c r="C9" s="40">
         <v>52.196249999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="41" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="39">
         <v>6500</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="40">
         <v>49.699599999999997</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="41" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="39">
         <v>7000</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="40">
         <v>52.242910000000002</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="41" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="39">
         <v>7500</v>
       </c>
-      <c r="C12" s="46">
+      <c r="C12" s="40">
         <v>52.756239999999998</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="41" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="39">
         <v>8000</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="40">
         <v>52.07958</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="39">
         <v>8500</v>
       </c>
-      <c r="C14" s="46">
+      <c r="C14" s="40">
         <v>51.636249999999997</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="41" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="39">
         <v>9000</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="40">
         <v>49.232939999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="41" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="39">
         <v>9500</v>
       </c>
-      <c r="C16" s="46">
+      <c r="C16" s="40">
         <v>47.926279999999998</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="41" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="39">
         <v>10000</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17" s="40">
         <v>48.20628</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="41" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="39">
         <v>10500</v>
       </c>
-      <c r="C18" s="46">
+      <c r="C18" s="40">
         <v>49.349600000000002</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="39">
         <v>11500</v>
       </c>
-      <c r="C19" s="46">
+      <c r="C19" s="40">
         <v>48.486280000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="41" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="39">
         <v>13000</v>
       </c>
-      <c r="C20" s="46">
+      <c r="C20" s="40">
         <v>47.342959999999998</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="41" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="39">
         <v>15000</v>
       </c>
-      <c r="C21" s="46">
+      <c r="C21" s="40">
         <v>42.699660000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bo y Resumen Performance update
</commit_message>
<xml_diff>
--- a/German/Resumen performance.xlsx
+++ b/German/Resumen performance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66681606-A769-408E-88B9-AB4FCC91C370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEED5F82-7B21-4E74-88DE-463BDE01D77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>N° intento</t>
   </si>
@@ -190,6 +190,21 @@
   <si>
     <t>De la clase 6, quinta  mejor bo del lgbm, con 15.000 envíos</t>
   </si>
+  <si>
+    <t>De la clase 7, mejor solucion del bo de lgbm de la carpeta  con 15000 envios</t>
+  </si>
+  <si>
+    <t>De la clase 7, segundo mejor solucion del bo de lgbm de la carpeta  con 15000 envios</t>
+  </si>
+  <si>
+    <t>De la clase 7, tercera mejor solucion del bo de lgbm de la carpeta  con 15000 envios</t>
+  </si>
+  <si>
+    <t>De la clase 7, cuarta mejor solucion del bo de lgbm de la carpeta  con 15000 envios</t>
+  </si>
+  <si>
+    <t>De la clase 7, quinta mejor solucion del bo de lgbm de la carpeta  con 15000 envios</t>
+  </si>
 </sst>
 </file>
 
@@ -201,7 +216,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +295,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -376,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -490,6 +511,7 @@
     <xf numFmtId="167" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -508,29 +530,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1323,7 +1332,7 @@
             <c:numRef>
               <c:f>'Segunda Competencia'!$H$3:$H$7</c:f>
               <c:numCache>
-                <c:formatCode>#.##000000</c:formatCode>
+                <c:formatCode>#,##0.00000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>96.251180000000005</c:v>
@@ -4509,10 +4518,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$B$3:$B$7</c:f>
+              <c:f>'Segunda Competencia'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4527,16 +4536,31 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$D$3:$D$7</c:f>
+              <c:f>'Segunda Competencia'!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>427</c:v>
                 </c:pt>
@@ -4551,6 +4575,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>62.524000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86.778999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86.495500000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>86.183999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85.991500000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85.581999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4589,10 +4628,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$B$3:$B$7</c:f>
+              <c:f>'Segunda Competencia'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4607,16 +4646,31 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$E$3:$E$7</c:f>
+              <c:f>'Segunda Competencia'!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>96.251180000000005</c:v>
                 </c:pt>
@@ -4631,6 +4685,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>142.87174999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>125.09153000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>141.89174</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.45158000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128.17157</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="#,##0">
+                  <c:v>139.65171000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4902,10 +4971,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$B$3:$B$7</c:f>
+              <c:f>'Segunda Competencia'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4920,16 +4989,31 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$F$3:$F$7</c:f>
+              <c:f>'Segunda Competencia'!$F$3:$F$12</c:f>
               <c:numCache>
-                <c:formatCode>#.##000000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>330.74882000000002</c:v>
                 </c:pt>
@@ -4944,6 +5028,18 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-80.347749999999991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-38.31253000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-55.396239999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-42.267580000000009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-42.180070000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5316,7 +5412,7 @@
             <c:numRef>
               <c:f>'Segunda Competencia'!$G$3:$G$7</c:f>
               <c:numCache>
-                <c:formatCode>#.##00000</c:formatCode>
+                <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
@@ -9196,7 +9292,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1065598</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>174650</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5610225" cy="3486150"/>
@@ -9229,13 +9325,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>280148</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>46423</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>563497</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>12806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9267,7 +9363,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>428626</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>102053</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5610225" cy="3486150"/>
@@ -9300,13 +9396,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>270783</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>554132</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>118784</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9622,41 +9718,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="42"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="46" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="7">
@@ -9679,7 +9775,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="8">
         <v>2</v>
       </c>
@@ -9705,7 +9801,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -9731,7 +9827,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -9757,7 +9853,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -9783,7 +9879,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="9">
         <v>6</v>
       </c>
@@ -9809,7 +9905,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="8">
         <v>7</v>
       </c>
@@ -9835,7 +9931,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -9861,7 +9957,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -9887,7 +9983,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -9913,7 +10009,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="9">
         <v>11</v>
       </c>
@@ -10565,17 +10661,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E6B357-D765-4AE5-80C2-9272AB64D6E1}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="12.5703125" style="1"/>
-    <col min="3" max="3" width="65.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
     <col min="6" max="7" width="25.7109375" style="1" customWidth="1"/>
@@ -10584,55 +10680,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="48"/>
-      <c r="B1" s="44" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44" t="s">
+      <c r="A2" s="41"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="42"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="10">
         <v>427</v>
       </c>
-      <c r="E3" s="53">
+      <c r="E3" s="10">
         <v>96.251180000000005</v>
       </c>
       <c r="F3" s="25">
@@ -10646,79 +10742,79 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="47">
+      <c r="A4" s="49"/>
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="53">
+      <c r="D4" s="10">
         <v>62.993000000000002</v>
       </c>
-      <c r="E4" s="53">
+      <c r="E4" s="10">
         <v>148.05180999999999</v>
       </c>
-      <c r="F4" s="54">
-        <f t="shared" ref="F4:F7" si="0">+D4-E4</f>
+      <c r="F4" s="26">
+        <f t="shared" ref="F4:F11" si="0">+D4-E4</f>
         <v>-85.058809999999994</v>
       </c>
-      <c r="G4" s="55"/>
-      <c r="H4" s="54">
-        <f t="shared" ref="H4:H7" si="1">+E4-G4</f>
+      <c r="G4" s="37"/>
+      <c r="H4" s="26">
+        <f t="shared" ref="H4:H11" si="1">+E4-G4</f>
         <v>148.05180999999999</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
-      <c r="B5" s="47">
+      <c r="A5" s="49"/>
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="10">
         <v>62.58</v>
       </c>
-      <c r="E5" s="53">
+      <c r="E5" s="10">
         <v>138.5317</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="26">
         <f t="shared" si="0"/>
         <v>-75.951700000000002</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="54">
+      <c r="G5" s="37"/>
+      <c r="H5" s="26">
         <f t="shared" si="1"/>
         <v>138.5317</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="47">
+      <c r="A6" s="49"/>
+      <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="10">
         <v>62.527500000000003</v>
       </c>
-      <c r="E6" s="53">
+      <c r="E6" s="10">
         <v>122.92151</v>
       </c>
-      <c r="F6" s="54">
+      <c r="F6" s="26">
         <f t="shared" si="0"/>
         <v>-60.394009999999994</v>
       </c>
-      <c r="G6" s="55"/>
-      <c r="H6" s="54">
+      <c r="G6" s="37"/>
+      <c r="H6" s="26">
         <f t="shared" si="1"/>
         <v>122.92151</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="9">
         <v>5</v>
       </c>
@@ -10740,6 +10836,115 @@
         <f t="shared" si="1"/>
         <v>142.87174999999999</v>
       </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="10">
+        <v>86.778999999999996</v>
+      </c>
+      <c r="E8" s="10">
+        <v>125.09153000000001</v>
+      </c>
+      <c r="F8" s="25">
+        <f t="shared" si="0"/>
+        <v>-38.31253000000001</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="25">
+        <f t="shared" si="1"/>
+        <v>125.09153000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="10">
+        <v>86.495500000000007</v>
+      </c>
+      <c r="E9" s="10">
+        <v>141.89174</v>
+      </c>
+      <c r="F9" s="26">
+        <f t="shared" si="0"/>
+        <v>-55.396239999999992</v>
+      </c>
+      <c r="G9" s="37"/>
+      <c r="H9" s="26">
+        <f t="shared" si="1"/>
+        <v>141.89174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="7">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="10">
+        <v>86.183999999999997</v>
+      </c>
+      <c r="E10" s="10">
+        <v>128.45158000000001</v>
+      </c>
+      <c r="F10" s="26">
+        <f t="shared" si="0"/>
+        <v>-42.267580000000009</v>
+      </c>
+      <c r="G10" s="37"/>
+      <c r="H10" s="26">
+        <f t="shared" si="1"/>
+        <v>128.45158000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="10">
+        <v>85.991500000000002</v>
+      </c>
+      <c r="E11" s="10">
+        <v>128.17157</v>
+      </c>
+      <c r="F11" s="26">
+        <f t="shared" si="0"/>
+        <v>-42.180070000000001</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="26">
+        <f t="shared" si="1"/>
+        <v>128.17157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>10</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="12">
+        <v>85.581999999999994</v>
+      </c>
+      <c r="E12" s="51">
+        <v>139.65171000000001</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="27"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:E7">

</xml_diff>

<commit_message>
Update performance competencia 2
</commit_message>
<xml_diff>
--- a/German/Resumen performance.xlsx
+++ b/German/Resumen performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Desktop\dmeyf2023\German\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28289A8-4935-45AC-8DF0-20B14F992442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED537387-2C0C-485E-8E61-CE64A62E42A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primera Competencia" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>N° intento</t>
   </si>
@@ -205,6 +205,9 @@
   <si>
     <t>De la clase 7, quinta mejor solucion del bo de lgbm de la carpeta  con 15000 envios</t>
   </si>
+  <si>
+    <t>FE  (drifing, ma, suma) y BO de LGBM</t>
+  </si>
 </sst>
 </file>
 
@@ -297,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +341,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -391,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -532,6 +541,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,96 +1260,72 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Primera Competencia'!$B$3:$B$24</c:f>
+              <c:f>'Segunda Competencia'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$H$3:$H$7</c:f>
+              <c:f>'Segunda Competencia'!$H$3:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00000</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>148.05180999999999</c:v>
+                  <c:v>22.94641</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>138.5317</c:v>
+                  <c:v>16.412959999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>122.92151</c:v>
+                  <c:v>-1.2427799999999962</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>142.87174999999999</c:v>
+                  <c:v>18.124129999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.6316499999999934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.7685699999999827</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.3649199999999837</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4128400000000028</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.8352100000000178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1462,8 +1450,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39831398120822664"/>
-          <c:y val="0.63289268282180655"/>
+          <c:x val="0.45083757093639637"/>
+          <c:y val="0.26039858553338763"/>
           <c:w val="0.54669776916299806"/>
           <c:h val="0.18760847726153632"/>
         </c:manualLayout>
@@ -4470,7 +4458,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.6194047475814245E-2"/>
+          <c:x val="8.1666599824427713E-2"/>
           <c:y val="0.12311719231817335"/>
           <c:w val="0.87915778778925979"/>
           <c:h val="0.79354531503234227"/>
@@ -5013,6 +5001,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-42.180070000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-54.069710000000015</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5269,9 +5260,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.7512666604280582E-2"/>
-          <c:y val="0.13040316681726261"/>
-          <c:w val="0.87915778778925979"/>
+          <c:x val="8.3125899585132487E-2"/>
+          <c:y val="0.12676017956771796"/>
+          <c:w val="0.91084992134896547"/>
           <c:h val="0.79354531503234227"/>
         </c:manualLayout>
       </c:layout>
@@ -5281,6 +5272,110 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Segunda Competencia'!$E$1:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Score 
+Kaggle Público</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Segunda Competencia'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Segunda Competencia'!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>148.05180999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.5317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122.92151</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>142.87174999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125.09153000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141.89174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128.45158000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.17157</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>139.65171000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BB56-4172-A476-E0882F0D240D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'Segunda Competencia'!$G$1:$G$2</c:f>
@@ -5305,218 +5400,72 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Primera Competencia'!$B$3:$B$25</c:f>
+              <c:f>'Segunda Competencia'!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Segunda Competencia'!$G$3:$G$7</c:f>
+              <c:f>'Segunda Competencia'!$G$3:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0000</c:formatCode>
-                <c:ptCount val="4"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BB56-4172-A476-E0882F0D240D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Segunda Competencia'!$E$1:$E$2</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>Score 
-Kaggle Público</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Primera Competencia'!$B$3:$B$25</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>125.10539999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>122.11874</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>124.16428999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>124.74762</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>126.72318</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>135.12317000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>133.81649999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>125.75873</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Segunda Competencia'!$E$3:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>148.05180999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>138.5317</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>122.92151</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>142.87174999999999</c:v>
+                  <c:v>133.81649999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5597,7 +5546,7 @@
         <c:axId val="1819361754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="10"/>
+          <c:min val="120"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -5654,8 +5603,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.56661720340984545"/>
-          <c:y val="0.60247235489006501"/>
+          <c:x val="0.62547402287787024"/>
+          <c:y val="0.1981007701906114"/>
           <c:w val="0.34283384356242397"/>
           <c:h val="0.19035669721612672"/>
         </c:manualLayout>
@@ -9293,16 +9242,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>280148</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>46423</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>806823</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1599</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>563497</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>12806</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>597114</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>158482</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9332,11 +9281,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>428626</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>102053</xdr:rowOff>
+      <xdr:colOff>989302</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5610225" cy="3486150"/>
+    <xdr:ext cx="5572123" cy="3602211"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 1" title="Gráfico">
@@ -9364,16 +9313,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>270783</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>922380</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>554132</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>118784</xdr:rowOff>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10633,8 +10582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E6B357-D765-4AE5-80C2-9272AB64D6E1}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10649,7 +10598,7 @@
     <col min="9" max="9" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="41"/>
       <c r="B1" s="45" t="s">
         <v>0</v>
@@ -10673,7 +10622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="41"/>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
@@ -10685,7 +10634,7 @@
       <c r="G2" s="45"/>
       <c r="H2" s="43"/>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>44</v>
       </c>
@@ -10705,13 +10654,19 @@
         <f>+D3-E3</f>
         <v>330.74882000000002</v>
       </c>
-      <c r="G3" s="38"/>
+      <c r="G3" s="38">
+        <v>106.90541999999999</v>
+      </c>
       <c r="H3" s="25">
         <f>+E3-G3</f>
-        <v>96.251180000000005</v>
+        <v>-10.654239999999987</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I2:I3" si="0">+G3/1000</f>
+        <v>0.10690541999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="49"/>
       <c r="B4" s="7">
         <v>2</v>
@@ -10726,16 +10681,18 @@
         <v>148.05180999999999</v>
       </c>
       <c r="F4" s="26">
-        <f t="shared" ref="F4:F11" si="0">+D4-E4</f>
+        <f t="shared" ref="F4:F12" si="1">+D4-E4</f>
         <v>-85.058809999999994</v>
       </c>
-      <c r="G4" s="37"/>
+      <c r="G4" s="37">
+        <v>125.10539999999999</v>
+      </c>
       <c r="H4" s="26">
-        <f t="shared" ref="H4:H11" si="1">+E4-G4</f>
-        <v>148.05180999999999</v>
+        <f t="shared" ref="H4:H12" si="2">+E4-G4</f>
+        <v>22.94641</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="7">
         <v>3</v>
@@ -10750,16 +10707,18 @@
         <v>138.5317</v>
       </c>
       <c r="F5" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-75.951700000000002</v>
       </c>
-      <c r="G5" s="37"/>
+      <c r="G5" s="37">
+        <v>122.11874</v>
+      </c>
       <c r="H5" s="26">
-        <f t="shared" si="1"/>
-        <v>138.5317</v>
+        <f t="shared" si="2"/>
+        <v>16.412959999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
       <c r="B6" s="7">
         <v>4</v>
@@ -10774,16 +10733,18 @@
         <v>122.92151</v>
       </c>
       <c r="F6" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-60.394009999999994</v>
       </c>
-      <c r="G6" s="37"/>
+      <c r="G6" s="37">
+        <v>124.16428999999999</v>
+      </c>
       <c r="H6" s="26">
-        <f t="shared" si="1"/>
-        <v>122.92151</v>
+        <f t="shared" si="2"/>
+        <v>-1.2427799999999962</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="50"/>
       <c r="B7" s="9">
         <v>5</v>
@@ -10798,16 +10759,21 @@
         <v>142.87174999999999</v>
       </c>
       <c r="F7" s="27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-80.347749999999991</v>
       </c>
-      <c r="G7" s="39"/>
+      <c r="G7" s="39">
+        <v>124.74762</v>
+      </c>
       <c r="H7" s="27">
-        <f t="shared" si="1"/>
-        <v>142.87174999999999</v>
+        <f t="shared" si="2"/>
+        <v>18.124129999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>54</v>
+      </c>
       <c r="B8" s="8">
         <v>6</v>
       </c>
@@ -10821,16 +10787,19 @@
         <v>125.09153000000001</v>
       </c>
       <c r="F8" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-38.31253000000001</v>
       </c>
-      <c r="G8" s="38"/>
+      <c r="G8" s="38">
+        <v>126.72318</v>
+      </c>
       <c r="H8" s="25">
-        <f t="shared" si="1"/>
-        <v>125.09153000000001</v>
+        <f t="shared" si="2"/>
+        <v>-1.6316499999999934</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -10844,16 +10813,19 @@
         <v>141.89174</v>
       </c>
       <c r="F9" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-55.396239999999992</v>
       </c>
-      <c r="G9" s="37"/>
+      <c r="G9" s="51">
+        <v>135.12317000000002</v>
+      </c>
       <c r="H9" s="26">
-        <f t="shared" si="1"/>
-        <v>141.89174</v>
+        <f t="shared" si="2"/>
+        <v>6.7685699999999827</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -10867,16 +10839,19 @@
         <v>128.45158000000001</v>
       </c>
       <c r="F10" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-42.267580000000009</v>
       </c>
-      <c r="G10" s="37"/>
+      <c r="G10" s="37">
+        <v>133.81649999999999</v>
+      </c>
       <c r="H10" s="26">
-        <f t="shared" si="1"/>
-        <v>128.45158000000001</v>
+        <f t="shared" si="2"/>
+        <v>-5.3649199999999837</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -10890,16 +10865,19 @@
         <v>128.17157</v>
       </c>
       <c r="F11" s="26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-42.180070000000001</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="37">
+        <v>125.75873</v>
+      </c>
       <c r="H11" s="26">
-        <f t="shared" si="1"/>
-        <v>128.17157</v>
+        <f t="shared" si="2"/>
+        <v>2.4128400000000028</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
       <c r="B12" s="9">
         <v>10</v>
       </c>
@@ -10912,15 +10890,24 @@
       <c r="E12" s="12">
         <v>139.65171000000001</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="27"/>
+      <c r="F12" s="27">
+        <f>+D12-E12</f>
+        <v>-54.069710000000015</v>
+      </c>
+      <c r="G12" s="39">
+        <v>133.81649999999999</v>
+      </c>
+      <c r="H12" s="27">
+        <f t="shared" si="2"/>
+        <v>5.8352100000000178</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:E7">
     <sortCondition descending="1" ref="E4:E7"/>
   </sortState>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A8:A12"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B1:B2"/>

</xml_diff>